<commit_message>
profile updated with extra works and extra etext
</commit_message>
<xml_diff>
--- a/data/philo_profiles/P0AT0383-སློབ་དཔོན་ཤཱཀྱ་འོད་.xlsx
+++ b/data/philo_profiles/P0AT0383-སློབ་དཔོན་ཤཱཀྱ་འོད་.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,262 +417,419 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
     <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>OCRability info</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Work</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Instance</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Cover</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B2">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3354","bdr:MW1PD95844_3354")</f>
-        <v/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cover Page</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Random Page</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extra work</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extra Etext</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="70" customHeight="1">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B3">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW22704_4415","bdr:MW22704_4415")</f>
-        <v/>
+      <c r="D2">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3354?uilang=bo","MW1PD95844_3354")</f>
+        <v/>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H2">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" ht="70" customHeight="1">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B4">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3357","bdr:MW1PD95844_3357")</f>
-        <v/>
+      <c r="D3">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW22704_4415?uilang=bo","MW22704_4415")</f>
+        <v/>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H3">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="70" customHeight="1">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B5">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23703_4124","bdr:MW23703_4124")</f>
-        <v/>
+      <c r="D4">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3357?uilang=bo","MW1PD95844_3357")</f>
+        <v/>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H4">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="70" customHeight="1">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B6">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23702_3629","bdr:MW23702_3629")</f>
-        <v/>
+      <c r="D5">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23703_4124?uilang=bo","MW23703_4124")</f>
+        <v/>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H5">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="70" customHeight="1">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B7">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1KG13126_5626","bdr:MW1KG13126_5626")</f>
-        <v/>
+      <c r="D6">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23702_3629?uilang=bo","MW23702_3629")</f>
+        <v/>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H6">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="70" customHeight="1">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3462</t>
-        </is>
-      </c>
-      <c r="B8">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW2KG5015_4415","bdr:MW2KG5015_4415")</f>
-        <v/>
+      <c r="D7">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1KG13126_5626?uilang=bo","MW1KG13126_5626")</f>
+        <v/>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H7">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="70" customHeight="1">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>WA0RT3462</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B9">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23702_3630","bdr:MW23702_3630")</f>
-        <v/>
+      <c r="D8">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW2KG5015_4415?uilang=bo","MW2KG5015_4415")</f>
+        <v/>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པ།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="70" customHeight="1">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>འཕགས་པ་ཐམས་ཅད་ཡོད་པར་སམར་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུ་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B10">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1KG13126_5627","bdr:MW1KG13126_5627")</f>
-        <v/>
+      <c r="D9">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23702_3630?uilang=bo","MW23702_3630")</f>
+        <v/>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་ཐམས་ཅད་ཡོད་པར་སམར་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུ་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H9">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་ཐམས་ཅད་ཡོད་པར་སམར་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུ་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="70" customHeight="1">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B11">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW2KG5015_4416","bdr:MW2KG5015_4416")</f>
-        <v/>
+      <c r="D10">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1KG13126_5627?uilang=bo","MW1KG13126_5627")</f>
+        <v/>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H10">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="70" customHeight="1">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B12">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW22704_4416","bdr:MW22704_4416")</f>
-        <v/>
+      <c r="D11">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW2KG5015_4416?uilang=bo","MW2KG5015_4416")</f>
+        <v/>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H11">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="70" customHeight="1">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B13">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23703_4125","bdr:MW23703_4125")</f>
-        <v/>
+      <c r="D12">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW22704_4416?uilang=bo","MW22704_4416")</f>
+        <v/>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H12">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" ht="70" customHeight="1">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>bdr:WA0RT3463</t>
-        </is>
-      </c>
-      <c r="B14">
-        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3355","bdr:MW1PD95844_3355")</f>
-        <v/>
+      <c r="D13">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW23703_4125?uilang=bo","MW23703_4125")</f>
+        <v/>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H13">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" ht="70" customHeight="1">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WA0RT3463</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14">
+        <f>HYPERLINK("https://library.bdrc.io/show/bdr:MW1PD95844_3355?uilang=bo","MW1PD95844_3355")</f>
+        <v/>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Work&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "བརྩམས་ཆོས་གཞན།")</f>
+        <v/>
+      </c>
+      <c r="H14">
+        <f>HYPERLINK("https://library.bdrc.io/search?lg=bo&amp;t=Etext&amp;pg=1&amp;f=author,exc,bdr:P0AT0383&amp;uilang=bo&amp;q=འཕགས་པ་གཞི་ཐམས་ཅད་ཡོད་པར་སྨྲ་བའི་དགེ་ཚུལ་གྱི་ཚིག་ལེའུར་བྱས་པའི་འགྲེལ་པ་འོད་ལྡན།~1", "ཡིག་རྐྱང་གཞན།")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>